<commit_message>
Complete paper first draft
</commit_message>
<xml_diff>
--- a/old_dont_use/training_data_metrics.xlsx
+++ b/old_dont_use/training_data_metrics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taylor\Documents\School\COMP4710\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taylor\Documents\School\COMP4710\old_dont_use\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>1900-2000</t>
   </si>
@@ -40,18 +39,6 @@
     <t>1950-2000</t>
   </si>
   <si>
-    <t>69.65 (65.72)</t>
-  </si>
-  <si>
-    <t>65.41 (60.83)</t>
-  </si>
-  <si>
-    <t>71.65 (63.63)</t>
-  </si>
-  <si>
-    <t>75.22 (67.33)</t>
-  </si>
-  <si>
     <t>Range</t>
   </si>
   <si>
@@ -73,9 +60,6 @@
     <t>AL111976</t>
   </si>
   <si>
-    <t>⟨ ⟩,</t>
-  </si>
-  <si>
     <t>⟨ (26.0:-84.0),(25.3:-83.3),(24.7:-82.7) ⟩</t>
   </si>
   <si>
@@ -86,6 +70,18 @@
   </si>
   <si>
     <t>⟨ (12.5:-37.5),(13.0:-39.0),(13.5:-40.5) ⟩</t>
+  </si>
+  <si>
+    <t>75.0 (72.58)</t>
+  </si>
+  <si>
+    <t>72.46 (69.93)</t>
+  </si>
+  <si>
+    <t>74.16 (71.77)</t>
+  </si>
+  <si>
+    <t>73.18 (70.62)</t>
   </si>
 </sst>
 </file>
@@ -136,10 +132,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,95 +434,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:H15"/>
+  <dimension ref="A4:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C14"/>
+      <selection activeCell="D20" sqref="B18:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D18" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="C20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H15" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>